<commit_message>
Demo 3 code is changed (non_storage is changed to non_storage_nodes in mass balance) pluse some max flow in input data. Now same results.
</commit_message>
<xml_diff>
--- a/tutorial/Demo_models/Demo3/Schematic of Network3.xlsx
+++ b/tutorial/Demo_models/Demo3/Schematic of Network3.xlsx
@@ -4374,321 +4374,6 @@
           </a:ext>
         </a:extLst>
       </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>54447</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>199227</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>155666</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="102" name="Oval 101"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3777361" y="1143000"/>
-          <a:ext cx="144780" cy="155666"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>174172</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>318952</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>155666</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="103" name="Oval 102"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5138058" y="0"/>
-          <a:ext cx="144780" cy="155666"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>446314</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>10886</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>591094</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>3266</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="104" name="Oval 103"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7892143" y="3276600"/>
-          <a:ext cx="144780" cy="155666"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>326571</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>214260</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="105" name="Text Box 91"/>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5290457" y="0"/>
-          <a:ext cx="508174" cy="191860"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF">
-            <a:alpha val="0"/>
-          </a:srgbClr>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="0" anchor="t" upright="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l" rtl="1">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>StartPt1</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>587829</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>108858</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>475518</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>137433</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="106" name="Text Box 91"/>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3690258" y="925287"/>
-          <a:ext cx="508174" cy="191860"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF">
-            <a:alpha val="0"/>
-          </a:srgbClr>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="0" anchor="t" upright="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l" rtl="1">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>StartPt2</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>508174</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="107" name="Text Box 91"/>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="8066314" y="3429000"/>
-          <a:ext cx="508174" cy="191860"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF">
-            <a:alpha val="0"/>
-          </a:srgbClr>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="0" bIns="0" anchor="t" upright="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l" rtl="1">
-            <a:defRPr sz="1000"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="0" i="0" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-              <a:cs typeface="Arial"/>
-            </a:rPr>
-            <a:t>StartPt3</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -4985,7 +4670,7 @@
   <dimension ref="B2:R22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>